<commit_message>
update taakverdeling & logboek
</commit_message>
<xml_diff>
--- a/Documentatie/Logboeken/Logboek-Luca-Joos.xlsx
+++ b/Documentatie/Logboeken/Logboek-Luca-Joos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project Fleet\Documentatie\Logboeken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EDCCA6-7ABA-4D93-81B5-9F53209CC6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5D0510-0BA6-437E-94B2-F7959840AB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8061FC93-56C2-42F0-A18D-5BD7334FDD21}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Beschrijving uitgevoerde taak</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Voertuig testen verbetert</t>
+  </si>
+  <si>
+    <t>Commentaar, properties en testen bij Tankaart</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -528,6 +531,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -844,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D6AFDB-6262-4F13-AC19-7AE452681B0C}">
   <dimension ref="D2:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,10 +1036,18 @@
       </c>
     </row>
     <row r="16" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="27"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="28"/>
+      <c r="D16" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="36">
+        <v>44490</v>
+      </c>
+      <c r="F16" s="26">
+        <v>2</v>
+      </c>
+      <c r="G16" s="28">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="33" t="s">
@@ -1041,8 +1055,8 @@
       </c>
       <c r="E17" s="34"/>
       <c r="F17" s="15">
-        <f>SUM(F5:F15)</f>
-        <v>23</v>
+        <f>SUM(F5:F16)</f>
+        <v>25</v>
       </c>
       <c r="G17" s="25">
         <f>SUM(G5:G12)</f>

</xml_diff>

<commit_message>
update logboek Luca /taakverdeling + parameter in methode BranstoftypeManager
</commit_message>
<xml_diff>
--- a/Documentatie/Logboeken/Logboek-Luca-Joos.xlsx
+++ b/Documentatie/Logboeken/Logboek-Luca-Joos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project Fleet\Documentatie\Logboeken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5D0510-0BA6-437E-94B2-F7959840AB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A6BAF6-DBD9-4A15-B5F5-0D69B8AD2845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8061FC93-56C2-42F0-A18D-5BD7334FDD21}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Beschrijving uitgevoerde taak</t>
   </si>
@@ -117,7 +117,10 @@
     <t>Voertuig testen verbetert</t>
   </si>
   <si>
-    <t>Commentaar, properties en testen bij Tankaart</t>
+    <t>Commentaar, properties, methode en testen bij Tankaart</t>
+  </si>
+  <si>
+    <t>Implementatie RijbewijsTypeRepo</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -286,32 +289,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -353,7 +330,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -362,73 +339,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -436,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -468,48 +378,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -530,10 +418,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -848,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D6AFDB-6262-4F13-AC19-7AE452681B0C}">
-  <dimension ref="D2:L17"/>
+  <dimension ref="D2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,12 +758,12 @@
   <sheetData>
     <row r="2" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="4:12" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="4:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D4" s="5" t="s">
@@ -878,27 +772,27 @@
       <c r="E4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="4">
         <v>44469</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <v>1.5</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="25" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2">
@@ -907,12 +801,12 @@
       <c r="F6" s="3">
         <v>1.5</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="26" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2">
@@ -921,10 +815,10 @@
       <c r="F7" s="3">
         <v>2</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="26" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2">
@@ -933,10 +827,10 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="4:12" s="8" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -945,12 +839,12 @@
       <c r="F9" s="7">
         <v>6</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="4:12" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="27" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -959,13 +853,13 @@
       <c r="F10" s="7">
         <v>4</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="7">
         <v>4</v>
       </c>
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="26" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="2">
@@ -974,24 +868,24 @@
       <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="4:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="2">
         <v>44483</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="3">
         <v>2</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="29">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="4:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="28" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="2">
@@ -1000,12 +894,12 @@
       <c r="F13" s="3">
         <v>3</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="29">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="4:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="2">
@@ -1014,7 +908,7 @@
       <c r="F14" s="3">
         <v>0.8</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="29">
         <v>0.8</v>
       </c>
       <c r="H14" t="s">
@@ -1022,7 +916,7 @@
       </c>
     </row>
     <row r="15" spans="4:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="2">
@@ -1031,34 +925,114 @@
       <c r="F15" s="3">
         <v>0.2</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="29">
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="27" t="s">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="2">
         <v>44490</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="3">
         <v>2</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="33" t="s">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2">
+        <v>44494</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="25"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="25"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="25"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="25"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="25"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="25"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="25"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="25"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="25"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D27" s="25"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="30"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="15">
-        <f>SUM(F5:F16)</f>
-        <v>25</v>
-      </c>
-      <c r="G17" s="25">
+      <c r="E29" s="24"/>
+      <c r="F29" s="13">
+        <f>SUM(F5:F17)</f>
+        <v>27</v>
+      </c>
+      <c r="G29" s="17">
         <f>SUM(G5:G12)</f>
         <v>13</v>
       </c>
@@ -1066,7 +1040,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>